<commit_message>
sprint 35 and configuration changes
</commit_message>
<xml_diff>
--- a/src/test/resources/fitchfieldID.xlsx
+++ b/src/test/resources/fitchfieldID.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="3018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3035" uniqueCount="3035">
   <si>
     <t>fitchFieldId</t>
   </si>
@@ -9070,6 +9070,57 @@
   </si>
   <si>
     <t>FC_DCR_SOLST</t>
+  </si>
+  <si>
+    <t>FC_OTHER_ADJ_NET_INC_RECONCILIATION_BNK</t>
+  </si>
+  <si>
+    <t>FC_PUBLISHED_NET_INCOME_BNK</t>
+  </si>
+  <si>
+    <t>FC_DEFER_TAX_ASSETS_DEDUCTED_CORE_CAPITAL_BNK</t>
+  </si>
+  <si>
+    <t>FC_INTANGIBLES_DEDUCTED_CORE_CAPITAL_BNK</t>
+  </si>
+  <si>
+    <t>FC_GROSS_PREM_WRITTEN_NONL_INS</t>
+  </si>
+  <si>
+    <t>FC_GROSS_PREM_WRITTEN_LIFE_INS</t>
+  </si>
+  <si>
+    <t>FC_GROSS_PREM_WRITTEN_REIN_NONL_INS</t>
+  </si>
+  <si>
+    <t>FC_GROSS_PREM_WRITTEN_REIN_LIFE_INS</t>
+  </si>
+  <si>
+    <t>FC_GROSS_PREM_WRITTEN_OTHER_INS</t>
+  </si>
+  <si>
+    <t>FC_GROSS_PREM_WRITTEN_CONS_ADJ_INS</t>
+  </si>
+  <si>
+    <t>FC_NET_PREM_WRITTEN_NONL_INS</t>
+  </si>
+  <si>
+    <t>FC_NET_PREM_WRITTEN_LIFE_INS</t>
+  </si>
+  <si>
+    <t>FC_NET_PREM_WRITTEN_REINS_NONL_INS</t>
+  </si>
+  <si>
+    <t>FC_NET_PREM_WRITTEN_REINS_LIFE_INS</t>
+  </si>
+  <si>
+    <t>FC_NET_PREM_WRITTEN_OTHER_INS</t>
+  </si>
+  <si>
+    <t>FC_NET_PREM_WRITTEN_CONS_ADJ_INS</t>
+  </si>
+  <si>
+    <t>FC_AUDITOR_NAME</t>
   </si>
 </sst>
 </file>
@@ -9538,10 +9589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3018"/>
+  <dimension ref="A1:A3035"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2979" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2992" sqref="F2992"/>
+    <sheetView tabSelected="1" topLeftCell="A2996" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3019" sqref="A3019"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24637,6 +24688,91 @@
     <row r="3018" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3018" s="10" t="s">
         <v>3017</v>
+      </c>
+    </row>
+    <row r="3019" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3019" s="3" t="s">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="3020" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3020" s="3" t="s">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="3021" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3021" s="3" t="s">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="3022" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3022" s="3" t="s">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="3023" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3023" s="3" t="s">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="3024" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3024" s="3" t="s">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="3025" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3025" s="3" t="s">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="3026" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3026" s="3" t="s">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="3027" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3027" s="3" t="s">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="3028" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3028" s="3" t="s">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="3029" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3029" s="3" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="3030" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3030" s="3" t="s">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="3031" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3031" s="3" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="3032" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3032" s="3" t="s">
+        <v>3031</v>
+      </c>
+    </row>
+    <row r="3033" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3033" s="3" t="s">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="3034" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3034" s="3" t="s">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="3035" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3035" s="3" t="s">
+        <v>3034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 5 content changes are updated and uploaded
</commit_message>
<xml_diff>
--- a/src/test/resources/fitchfieldID.xlsx
+++ b/src/test/resources/fitchfieldID.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$3289</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3415" uniqueCount="3339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3589" uniqueCount="3388">
   <si>
     <t>fitchFieldId</t>
   </si>
@@ -10055,6 +10055,153 @@
   </si>
   <si>
     <t>FC_SPONSOR_SPV</t>
+  </si>
+  <si>
+    <t>FC_ISSUER_NAME</t>
+  </si>
+  <si>
+    <t>FC_ISSUER_TYPE_DESC</t>
+  </si>
+  <si>
+    <t>FC_CVB_FLAG</t>
+  </si>
+  <si>
+    <t>FC_ELTR</t>
+  </si>
+  <si>
+    <t>FC_ELTR_ACTN</t>
+  </si>
+  <si>
+    <t>FC_ELTR_DT</t>
+  </si>
+  <si>
+    <t>FC_ELTR_ALRT</t>
+  </si>
+  <si>
+    <t>FC_ELTR_SOLST</t>
+  </si>
+  <si>
+    <t>FC_ESTR</t>
+  </si>
+  <si>
+    <t>FC_ESTR_ACTN</t>
+  </si>
+  <si>
+    <t>FC_ESTR_DT</t>
+  </si>
+  <si>
+    <t>FC_ESTR_ALRT</t>
+  </si>
+  <si>
+    <t>FC_ESTR_SOLST</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_GLOBAL_RANK</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_GLOBAL_RANK_CHG</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_COUNTRY_RANK</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_COUNTRY_RANK_CHG</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_RANK_VALUE</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_RANK_VALUE_CHG</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_RANK_STMT_DATE</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_RANK_ACCT_STANDARD</t>
+  </si>
+  <si>
+    <t>FC_OPERATING_PROFIT_RANK_CONS</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_GLOBAL_RANK</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_GLOBAL_RANK_CHG</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_COUNTRY_RANK</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_COUNTRY_RANK_CHG</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_RANK_VALUE</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_RANK_VALUE_CHG</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_RANK_STMT_DATE</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_RANK_ACCT_STANDARD</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSET_RANK_CONS</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_GLOBAL_RANK</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_GLOBAL_RANK_CHG</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_COUNTRY_RANK</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_COUNTRY_RANK_CHG</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_RANK_VALUE</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_RANK_VALUE_CHG</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_RANK_STMT_DATE</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_RANK_ACCT_STANDARD</t>
+  </si>
+  <si>
+    <t>FC_TIER1_CAPITAL_RANK_CONS</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_GLOBAL_RANK</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_GLOBAL_RANK_CHG</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_COUNTRY_RANK</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_COUNTRY_RANK_CHG</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_RANK_VALUE</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_RANK_VALUE_CHG</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_RANK_STMT_DATE</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_RANK_ACCT_STANDARD</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_WEIGHTED_RISK_RANK_CONS</t>
   </si>
 </sst>
 </file>
@@ -10146,7 +10293,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -10163,13 +10310,60 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -10584,10 +10778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3415"/>
+  <dimension ref="A1:A3589"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3261" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3290" sqref="D3290"/>
+    <sheetView tabSelected="1" topLeftCell="A3540" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3554" sqref="B3554:B3589"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27671,46 +27865,925 @@
         <v>3337</v>
       </c>
     </row>
+    <row r="3416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3416" s="9" t="s">
+        <v>3213</v>
+      </c>
+    </row>
+    <row r="3417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3417" s="9" t="s">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="3418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3418" s="9" t="s">
+        <v>3215</v>
+      </c>
+    </row>
+    <row r="3419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3419" s="9" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="3420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3420" s="9" t="s">
+        <v>3217</v>
+      </c>
+    </row>
+    <row r="3421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3421" s="9" t="s">
+        <v>3218</v>
+      </c>
+    </row>
+    <row r="3422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3422" s="9" t="s">
+        <v>3219</v>
+      </c>
+    </row>
+    <row r="3423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3423" s="9" t="s">
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="3424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3424" s="9" t="s">
+        <v>3221</v>
+      </c>
+    </row>
+    <row r="3425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3425" s="9" t="s">
+        <v>3222</v>
+      </c>
+    </row>
+    <row r="3426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3426" s="9" t="s">
+        <v>3223</v>
+      </c>
+    </row>
+    <row r="3427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3427" s="9" t="s">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="3428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3428" s="9" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="3429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3429" s="9" t="s">
+        <v>3226</v>
+      </c>
+    </row>
+    <row r="3430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3430" s="9" t="s">
+        <v>3227</v>
+      </c>
+    </row>
+    <row r="3431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3431" s="9" t="s">
+        <v>3228</v>
+      </c>
+    </row>
+    <row r="3432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3432" s="9" t="s">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="3433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3433" s="9" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="3434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3434" s="9" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="3435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3435" s="9" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="3436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3436" s="9" t="s">
+        <v>3233</v>
+      </c>
+    </row>
+    <row r="3437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3437" s="9" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="3438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3438" s="9" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="3439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3439" s="9" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="3440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3440" s="9" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="3441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3441" s="9" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="3442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3442" s="9" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3443" s="9" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="3444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3444" s="9" t="s">
+        <v>3241</v>
+      </c>
+    </row>
+    <row r="3445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3445" s="9" t="s">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="3446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3446" s="9" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="3447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3447" s="9" t="s">
+        <v>3244</v>
+      </c>
+    </row>
+    <row r="3448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3448" s="9" t="s">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="3449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3449" s="9" t="s">
+        <v>3246</v>
+      </c>
+    </row>
+    <row r="3450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3450" s="9" t="s">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="3451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3451" s="9" t="s">
+        <v>3248</v>
+      </c>
+    </row>
+    <row r="3452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3452" s="9" t="s">
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="3453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3453" s="9" t="s">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="3454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3454" s="9" t="s">
+        <v>3251</v>
+      </c>
+    </row>
+    <row r="3455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3455" s="9" t="s">
+        <v>3252</v>
+      </c>
+    </row>
+    <row r="3456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3456" s="9" t="s">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="3457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3457" s="9" t="s">
+        <v>3254</v>
+      </c>
+    </row>
+    <row r="3458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3458" s="9" t="s">
+        <v>3255</v>
+      </c>
+    </row>
+    <row r="3459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3459" s="9" t="s">
+        <v>3256</v>
+      </c>
+    </row>
+    <row r="3460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3460" s="9" t="s">
+        <v>3257</v>
+      </c>
+    </row>
+    <row r="3461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3461" s="9" t="s">
+        <v>3258</v>
+      </c>
+    </row>
+    <row r="3462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3462" s="9" t="s">
+        <v>3259</v>
+      </c>
+    </row>
+    <row r="3463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3463" s="9" t="s">
+        <v>3260</v>
+      </c>
+    </row>
+    <row r="3464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3464" s="9" t="s">
+        <v>3261</v>
+      </c>
+    </row>
+    <row r="3465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3465" s="9" t="s">
+        <v>3262</v>
+      </c>
+    </row>
+    <row r="3466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3466" s="9" t="s">
+        <v>3263</v>
+      </c>
+    </row>
+    <row r="3467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3467" s="9" t="s">
+        <v>3264</v>
+      </c>
+    </row>
+    <row r="3468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3468" s="9" t="s">
+        <v>3265</v>
+      </c>
+    </row>
+    <row r="3469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3469" s="9" t="s">
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="3470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3470" s="9" t="s">
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="3471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3471" s="9" t="s">
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="3472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3472" s="9" t="s">
+        <v>3269</v>
+      </c>
+    </row>
+    <row r="3473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3473" s="9" t="s">
+        <v>3270</v>
+      </c>
+    </row>
+    <row r="3474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3474" s="9" t="s">
+        <v>3271</v>
+      </c>
+    </row>
+    <row r="3475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3475" s="9" t="s">
+        <v>3272</v>
+      </c>
+    </row>
+    <row r="3476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3476" s="9" t="s">
+        <v>3273</v>
+      </c>
+    </row>
+    <row r="3477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3477" s="9" t="s">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="3478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3478" s="9" t="s">
+        <v>3275</v>
+      </c>
+    </row>
+    <row r="3479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3479" s="9" t="s">
+        <v>3276</v>
+      </c>
+    </row>
+    <row r="3480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3480" s="9" t="s">
+        <v>3277</v>
+      </c>
+    </row>
+    <row r="3481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3481" s="9" t="s">
+        <v>3278</v>
+      </c>
+    </row>
+    <row r="3482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3482" s="9" t="s">
+        <v>3279</v>
+      </c>
+    </row>
+    <row r="3483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3483" s="9" t="s">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="3484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3484" s="9" t="s">
+        <v>3281</v>
+      </c>
+    </row>
+    <row r="3485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3485" s="9" t="s">
+        <v>3282</v>
+      </c>
+    </row>
+    <row r="3486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3486" s="9" t="s">
+        <v>3283</v>
+      </c>
+    </row>
+    <row r="3487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3487" s="9" t="s">
+        <v>3284</v>
+      </c>
+    </row>
+    <row r="3488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3488" s="9" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="3489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3489" s="9" t="s">
+        <v>3286</v>
+      </c>
+    </row>
+    <row r="3490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3490" s="9" t="s">
+        <v>3287</v>
+      </c>
+    </row>
+    <row r="3491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3491" s="9" t="s">
+        <v>3288</v>
+      </c>
+    </row>
+    <row r="3492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3492" s="9" t="s">
+        <v>3289</v>
+      </c>
+    </row>
+    <row r="3493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3493" s="9" t="s">
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="3494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3494" s="9" t="s">
+        <v>3291</v>
+      </c>
+    </row>
+    <row r="3495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3495" s="9" t="s">
+        <v>3292</v>
+      </c>
+    </row>
+    <row r="3496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3496" s="9" t="s">
+        <v>3293</v>
+      </c>
+    </row>
+    <row r="3497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3497" s="9" t="s">
+        <v>3294</v>
+      </c>
+    </row>
+    <row r="3498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3498" s="9" t="s">
+        <v>3295</v>
+      </c>
+    </row>
+    <row r="3499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3499" s="9" t="s">
+        <v>3296</v>
+      </c>
+    </row>
+    <row r="3500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3500" s="9" t="s">
+        <v>3297</v>
+      </c>
+    </row>
+    <row r="3501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3501" s="9" t="s">
+        <v>3298</v>
+      </c>
+    </row>
+    <row r="3502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3502" s="9" t="s">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="3503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3503" s="9" t="s">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="3504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3504" s="9" t="s">
+        <v>3301</v>
+      </c>
+    </row>
+    <row r="3505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3505" s="9" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="3506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3506" s="9" t="s">
+        <v>3303</v>
+      </c>
+    </row>
+    <row r="3507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3507" s="9" t="s">
+        <v>3304</v>
+      </c>
+    </row>
+    <row r="3508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3508" s="9" t="s">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="3509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3509" s="9" t="s">
+        <v>3306</v>
+      </c>
+    </row>
+    <row r="3510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3510" s="9" t="s">
+        <v>3307</v>
+      </c>
+    </row>
+    <row r="3511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3511" s="9" t="s">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="3512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3512" s="9" t="s">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="3513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3513" s="9" t="s">
+        <v>3310</v>
+      </c>
+    </row>
+    <row r="3514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3514" s="9" t="s">
+        <v>3311</v>
+      </c>
+    </row>
+    <row r="3515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3515" s="9" t="s">
+        <v>3312</v>
+      </c>
+    </row>
+    <row r="3516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3516" s="9" t="s">
+        <v>3313</v>
+      </c>
+    </row>
+    <row r="3517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3517" s="9" t="s">
+        <v>3314</v>
+      </c>
+    </row>
+    <row r="3518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3518" s="9" t="s">
+        <v>3315</v>
+      </c>
+    </row>
+    <row r="3519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3519" s="9" t="s">
+        <v>3316</v>
+      </c>
+    </row>
+    <row r="3520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3520" s="9" t="s">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="3521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3521" s="9" t="s">
+        <v>3318</v>
+      </c>
+    </row>
+    <row r="3522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3522" s="9" t="s">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="3523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3523" s="9" t="s">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="3524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3524" s="9" t="s">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="3525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3525" s="9" t="s">
+        <v>3322</v>
+      </c>
+    </row>
+    <row r="3526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3526" s="9" t="s">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="3527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3527" s="9" t="s">
+        <v>3324</v>
+      </c>
+    </row>
+    <row r="3528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3528" s="9" t="s">
+        <v>3325</v>
+      </c>
+    </row>
+    <row r="3529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3529" s="9" t="s">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="3530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3530" s="9" t="s">
+        <v>3327</v>
+      </c>
+    </row>
+    <row r="3531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3531" s="9" t="s">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="3532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3532" s="9" t="s">
+        <v>3329</v>
+      </c>
+    </row>
+    <row r="3533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3533" s="9" t="s">
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="3534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3534" s="9" t="s">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="3535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3535" s="9" t="s">
+        <v>3332</v>
+      </c>
+    </row>
+    <row r="3536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3536" s="9" t="s">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="3537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3537" s="9" t="s">
+        <v>3334</v>
+      </c>
+    </row>
+    <row r="3538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3538" s="9" t="s">
+        <v>3335</v>
+      </c>
+    </row>
+    <row r="3539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3539" s="9" t="s">
+        <v>3336</v>
+      </c>
+    </row>
+    <row r="3540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3540" s="9" t="s">
+        <v>3337</v>
+      </c>
+    </row>
+    <row r="3541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3541" s="9" t="s">
+        <v>3339</v>
+      </c>
+    </row>
+    <row r="3542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3542" s="9" t="s">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="3543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3543" s="9" t="s">
+        <v>3341</v>
+      </c>
+    </row>
+    <row r="3544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3544" s="14" t="s">
+        <v>3342</v>
+      </c>
+    </row>
+    <row r="3545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3545" s="14" t="s">
+        <v>3343</v>
+      </c>
+    </row>
+    <row r="3546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3546" s="11" t="s">
+        <v>3344</v>
+      </c>
+    </row>
+    <row r="3547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3547" s="11" t="s">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="3548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3548" s="14" t="s">
+        <v>3346</v>
+      </c>
+    </row>
+    <row r="3549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3549" s="14" t="s">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="3550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3550" s="14" t="s">
+        <v>3348</v>
+      </c>
+    </row>
+    <row r="3551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3551" s="11" t="s">
+        <v>3349</v>
+      </c>
+    </row>
+    <row r="3552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3552" s="11" t="s">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="3553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3553" s="14" t="s">
+        <v>3351</v>
+      </c>
+    </row>
+    <row r="3554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3554" s="4" t="s">
+        <v>3352</v>
+      </c>
+    </row>
+    <row r="3555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3555" s="4" t="s">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="3556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3556" s="4" t="s">
+        <v>3354</v>
+      </c>
+    </row>
+    <row r="3557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3557" s="4" t="s">
+        <v>3355</v>
+      </c>
+    </row>
+    <row r="3558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3558" s="4" t="s">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="3559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3559" s="4" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="3560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3560" s="4" t="s">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="3561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3561" s="4" t="s">
+        <v>3359</v>
+      </c>
+    </row>
+    <row r="3562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3562" s="4" t="s">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="3563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3563" s="4" t="s">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="3564" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3564" s="4" t="s">
+        <v>3362</v>
+      </c>
+    </row>
+    <row r="3565" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3565" s="4" t="s">
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="3566" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3566" s="4" t="s">
+        <v>3364</v>
+      </c>
+    </row>
+    <row r="3567" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3567" s="4" t="s">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="3568" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3568" s="4" t="s">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="3569" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3569" s="4" t="s">
+        <v>3367</v>
+      </c>
+    </row>
+    <row r="3570" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3570" s="4" t="s">
+        <v>3368</v>
+      </c>
+    </row>
+    <row r="3571" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3571" s="4" t="s">
+        <v>3369</v>
+      </c>
+    </row>
+    <row r="3572" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3572" s="4" t="s">
+        <v>3370</v>
+      </c>
+    </row>
+    <row r="3573" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3573" s="4" t="s">
+        <v>3371</v>
+      </c>
+    </row>
+    <row r="3574" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3574" s="4" t="s">
+        <v>3372</v>
+      </c>
+    </row>
+    <row r="3575" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3575" s="4" t="s">
+        <v>3373</v>
+      </c>
+    </row>
+    <row r="3576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3576" s="4" t="s">
+        <v>3374</v>
+      </c>
+    </row>
+    <row r="3577" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3577" s="4" t="s">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="3578" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3578" s="4" t="s">
+        <v>3376</v>
+      </c>
+    </row>
+    <row r="3579" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3579" s="4" t="s">
+        <v>3377</v>
+      </c>
+    </row>
+    <row r="3580" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3580" s="4" t="s">
+        <v>3378</v>
+      </c>
+    </row>
+    <row r="3581" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3581" s="4" t="s">
+        <v>3379</v>
+      </c>
+    </row>
+    <row r="3582" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3582" s="4" t="s">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="3583" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3583" s="4" t="s">
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="3584" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3584" s="4" t="s">
+        <v>3382</v>
+      </c>
+    </row>
+    <row r="3585" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3585" s="4" t="s">
+        <v>3383</v>
+      </c>
+    </row>
+    <row r="3586" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3586" s="4" t="s">
+        <v>3384</v>
+      </c>
+    </row>
+    <row r="3587" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3587" s="4" t="s">
+        <v>3385</v>
+      </c>
+    </row>
+    <row r="3588" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3588" s="4" t="s">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="3589" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3589" s="4" t="s">
+        <v>3387</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A3289"/>
   <conditionalFormatting sqref="A34">
-    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2465:A2475">
-    <cfRule type="expression" dxfId="11" priority="22">
+    <cfRule type="expression" dxfId="16" priority="25">
       <formula>IF(FIND(" ",$E2465)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="10" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2476:A2757">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>IF(FIND(" ",$E2476)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2994:A3082">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>IF(FIND(" ",$E2994)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3083:A3290">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>IF(FIND(" ",$E3083)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2212">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>IF(FIND(" ",$E2212)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2211 A2758:A2983 A2986:A2993 A3291:A1048576 A2213:A2464">
-    <cfRule type="expression" dxfId="1" priority="72">
+  <conditionalFormatting sqref="A1:A2211 A2758:A2983 A2986:A2993 A3291:A3415 A2213:A2464 A3590:A1048576">
+    <cfRule type="expression" dxfId="6" priority="75">
       <formula>IF(FIND(" ",$E1)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="76"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3416:A3553">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3554:A3589">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>IF(FIND(" ",$E3554)&gt;0,TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
content Sprint 6, 7 ,8 Stories
</commit_message>
<xml_diff>
--- a/src/test/resources/fitchfieldID.xlsx
+++ b/src/test/resources/fitchfieldID.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3589" uniqueCount="3388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="3426">
   <si>
     <t>fitchFieldId</t>
   </si>
@@ -10202,6 +10202,120 @@
   </si>
   <si>
     <t>FC_TOTAL_WEIGHTED_RISK_RANK_CONS</t>
+  </si>
+  <si>
+    <t>FC_PERIOD_DT_FIR</t>
+  </si>
+  <si>
+    <t>FC_STATEMENT_ID_FIR</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSETS_FIR</t>
+  </si>
+  <si>
+    <t>FC_COUNTRY_RISK_IND_FIR</t>
+  </si>
+  <si>
+    <t>FC_REGION_FIR</t>
+  </si>
+  <si>
+    <t>FC_PERIOD_DT_RANK_FIR</t>
+  </si>
+  <si>
+    <t>FC_PROFIT_FIR</t>
+  </si>
+  <si>
+    <t>FC_LOAN_QUAL_FIR</t>
+  </si>
+  <si>
+    <t>FC_MODEL_SCORE_FIR</t>
+  </si>
+  <si>
+    <t>FC_FIR</t>
+  </si>
+  <si>
+    <t>FC_BAND_RANK_FIR</t>
+  </si>
+  <si>
+    <t>FC_PROFIT_CUTOFF_LOW_FIR</t>
+  </si>
+  <si>
+    <t>FC_PROFIT_CUTOFF_HIGH_FIR</t>
+  </si>
+  <si>
+    <t>FC_LOAN_QUAL_CUTOFF_LOW_FIR</t>
+  </si>
+  <si>
+    <t>FC_LOAN_QUAL_CUTOFF_HIGH_FIR</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSETS_NORM_MEAN_FIR</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSETS_NORM_SD_FIR</t>
+  </si>
+  <si>
+    <t>FC_PROFIT_NORM_MEAN_FIR</t>
+  </si>
+  <si>
+    <t>FC_PROFIT_NORM_SD_FIR</t>
+  </si>
+  <si>
+    <t>FC_LOAN_QUAL_NORM_MEAN_FIR</t>
+  </si>
+  <si>
+    <t>FC_LOAN_QUAL_NORM_SD_FIR</t>
+  </si>
+  <si>
+    <t>FC_PROFIT_COEFF_FIR</t>
+  </si>
+  <si>
+    <t>FC_LOAN_QUAL_COEFF_FIR</t>
+  </si>
+  <si>
+    <t>FC_TOTAL_ASSETS_COEFF_FIR</t>
+  </si>
+  <si>
+    <t>FC_CRI_MODEL_COEFF_FIR</t>
+  </si>
+  <si>
+    <t>FC_INTERCEPTS_NO_FIR</t>
+  </si>
+  <si>
+    <t>FC_INTERCEPTS_FIR</t>
+  </si>
+  <si>
+    <t>FC_MIN_MODEL_SCORE_FIR</t>
+  </si>
+  <si>
+    <t>FC_MAX_MODEL_SCORE_FIR</t>
+  </si>
+  <si>
+    <t>FC_NOTCH_DIFF_ALL_FIR</t>
+  </si>
+  <si>
+    <t>FC_ENTITIES_NOTCH_DIFF_ALL_FIR</t>
+  </si>
+  <si>
+    <t>FC_NOTCH_DIFF_CF_ALL_FIR</t>
+  </si>
+  <si>
+    <t>FC_NOTCH_DIFF_EM_FIR</t>
+  </si>
+  <si>
+    <t>FC_ENTITIES_NOTCH_DIFF_EM_FIR</t>
+  </si>
+  <si>
+    <t>FC_NOTCH_DIFF_CF_EM_FIR</t>
+  </si>
+  <si>
+    <t>FC_NOTCH_DIFF_DM_FIR</t>
+  </si>
+  <si>
+    <t>FC_ENTITIES_NOTCH_DIFF_DM_FIR</t>
+  </si>
+  <si>
+    <t>FC_NOTCH_DIFF_CF_DM_FIR</t>
   </si>
 </sst>
 </file>
@@ -10319,24 +10433,7 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -10778,10 +10875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3589"/>
+  <dimension ref="A1:A3627"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3540" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3554" sqref="B3554:B3589"/>
+    <sheetView tabSelected="1" topLeftCell="A3597" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3599" sqref="D3599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28735,55 +28832,245 @@
         <v>3387</v>
       </c>
     </row>
+    <row r="3590" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3590" s="3" t="s">
+        <v>3388</v>
+      </c>
+    </row>
+    <row r="3591" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3591" s="3" t="s">
+        <v>3389</v>
+      </c>
+    </row>
+    <row r="3592" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3592" s="3" t="s">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="3593" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3593" s="3" t="s">
+        <v>3391</v>
+      </c>
+    </row>
+    <row r="3594" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3594" s="3" t="s">
+        <v>3392</v>
+      </c>
+    </row>
+    <row r="3595" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3595" s="3" t="s">
+        <v>3393</v>
+      </c>
+    </row>
+    <row r="3596" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3596" s="3" t="s">
+        <v>3394</v>
+      </c>
+    </row>
+    <row r="3597" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3597" s="3" t="s">
+        <v>3395</v>
+      </c>
+    </row>
+    <row r="3598" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3598" s="3" t="s">
+        <v>3396</v>
+      </c>
+    </row>
+    <row r="3599" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3599" s="3" t="s">
+        <v>3397</v>
+      </c>
+    </row>
+    <row r="3600" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3600" s="3" t="s">
+        <v>3398</v>
+      </c>
+    </row>
+    <row r="3601" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3601" s="3" t="s">
+        <v>3399</v>
+      </c>
+    </row>
+    <row r="3602" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3602" s="3" t="s">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="3603" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3603" s="3" t="s">
+        <v>3401</v>
+      </c>
+    </row>
+    <row r="3604" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3604" s="3" t="s">
+        <v>3402</v>
+      </c>
+    </row>
+    <row r="3605" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3605" s="3" t="s">
+        <v>3403</v>
+      </c>
+    </row>
+    <row r="3606" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3606" s="3" t="s">
+        <v>3404</v>
+      </c>
+    </row>
+    <row r="3607" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3607" s="3" t="s">
+        <v>3405</v>
+      </c>
+    </row>
+    <row r="3608" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3608" s="3" t="s">
+        <v>3406</v>
+      </c>
+    </row>
+    <row r="3609" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3609" s="3" t="s">
+        <v>3407</v>
+      </c>
+    </row>
+    <row r="3610" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3610" s="3" t="s">
+        <v>3408</v>
+      </c>
+    </row>
+    <row r="3611" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3611" s="3" t="s">
+        <v>3409</v>
+      </c>
+    </row>
+    <row r="3612" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3612" s="3" t="s">
+        <v>3410</v>
+      </c>
+    </row>
+    <row r="3613" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3613" s="3" t="s">
+        <v>3411</v>
+      </c>
+    </row>
+    <row r="3614" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3614" s="3" t="s">
+        <v>3412</v>
+      </c>
+    </row>
+    <row r="3615" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3615" s="3" t="s">
+        <v>3413</v>
+      </c>
+    </row>
+    <row r="3616" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3616" s="3" t="s">
+        <v>3414</v>
+      </c>
+    </row>
+    <row r="3617" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3617" s="3" t="s">
+        <v>3415</v>
+      </c>
+    </row>
+    <row r="3618" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3618" s="3" t="s">
+        <v>3416</v>
+      </c>
+    </row>
+    <row r="3619" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3619" s="3" t="s">
+        <v>3417</v>
+      </c>
+    </row>
+    <row r="3620" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3620" s="3" t="s">
+        <v>3418</v>
+      </c>
+    </row>
+    <row r="3621" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3621" s="3" t="s">
+        <v>3419</v>
+      </c>
+    </row>
+    <row r="3622" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3622" s="3" t="s">
+        <v>3420</v>
+      </c>
+    </row>
+    <row r="3623" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3623" s="3" t="s">
+        <v>3421</v>
+      </c>
+    </row>
+    <row r="3624" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3624" s="3" t="s">
+        <v>3422</v>
+      </c>
+    </row>
+    <row r="3625" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3625" s="3" t="s">
+        <v>3423</v>
+      </c>
+    </row>
+    <row r="3626" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3626" s="3" t="s">
+        <v>3424</v>
+      </c>
+    </row>
+    <row r="3627" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3627" s="3" t="s">
+        <v>3425</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A3289"/>
   <conditionalFormatting sqref="A34">
-    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2465:A2475">
-    <cfRule type="expression" dxfId="16" priority="25">
+    <cfRule type="expression" dxfId="14" priority="25">
       <formula>IF(FIND(" ",$E2465)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="15" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2476:A2757">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>IF(FIND(" ",$E2476)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2994:A3082">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>IF(FIND(" ",$E2994)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3083:A3290">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>IF(FIND(" ",$E3083)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2212">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>IF(FIND(" ",$E2212)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A2211 A2758:A2983 A2986:A2993 A3291:A3415 A2213:A2464 A3590:A1048576">
-    <cfRule type="expression" dxfId="6" priority="75">
+    <cfRule type="expression" dxfId="4" priority="75">
       <formula>IF(FIND(" ",$E1)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="5" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3416:A3553">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3554:A3589">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF(FIND(" ",$E3554)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sprint 9 Test cases added
</commit_message>
<xml_diff>
--- a/src/test/resources/fitchfieldID.xlsx
+++ b/src/test/resources/fitchfieldID.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$3289</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterate="1" calcOnSave="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="3426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3600" uniqueCount="3399">
   <si>
     <t>fitchFieldId</t>
   </si>
@@ -10235,87 +10235,6 @@
   </si>
   <si>
     <t>FC_BAND_RANK_FIR</t>
-  </si>
-  <si>
-    <t>FC_PROFIT_CUTOFF_LOW_FIR</t>
-  </si>
-  <si>
-    <t>FC_PROFIT_CUTOFF_HIGH_FIR</t>
-  </si>
-  <si>
-    <t>FC_LOAN_QUAL_CUTOFF_LOW_FIR</t>
-  </si>
-  <si>
-    <t>FC_LOAN_QUAL_CUTOFF_HIGH_FIR</t>
-  </si>
-  <si>
-    <t>FC_TOTAL_ASSETS_NORM_MEAN_FIR</t>
-  </si>
-  <si>
-    <t>FC_TOTAL_ASSETS_NORM_SD_FIR</t>
-  </si>
-  <si>
-    <t>FC_PROFIT_NORM_MEAN_FIR</t>
-  </si>
-  <si>
-    <t>FC_PROFIT_NORM_SD_FIR</t>
-  </si>
-  <si>
-    <t>FC_LOAN_QUAL_NORM_MEAN_FIR</t>
-  </si>
-  <si>
-    <t>FC_LOAN_QUAL_NORM_SD_FIR</t>
-  </si>
-  <si>
-    <t>FC_PROFIT_COEFF_FIR</t>
-  </si>
-  <si>
-    <t>FC_LOAN_QUAL_COEFF_FIR</t>
-  </si>
-  <si>
-    <t>FC_TOTAL_ASSETS_COEFF_FIR</t>
-  </si>
-  <si>
-    <t>FC_CRI_MODEL_COEFF_FIR</t>
-  </si>
-  <si>
-    <t>FC_INTERCEPTS_NO_FIR</t>
-  </si>
-  <si>
-    <t>FC_INTERCEPTS_FIR</t>
-  </si>
-  <si>
-    <t>FC_MIN_MODEL_SCORE_FIR</t>
-  </si>
-  <si>
-    <t>FC_MAX_MODEL_SCORE_FIR</t>
-  </si>
-  <si>
-    <t>FC_NOTCH_DIFF_ALL_FIR</t>
-  </si>
-  <si>
-    <t>FC_ENTITIES_NOTCH_DIFF_ALL_FIR</t>
-  </si>
-  <si>
-    <t>FC_NOTCH_DIFF_CF_ALL_FIR</t>
-  </si>
-  <si>
-    <t>FC_NOTCH_DIFF_EM_FIR</t>
-  </si>
-  <si>
-    <t>FC_ENTITIES_NOTCH_DIFF_EM_FIR</t>
-  </si>
-  <si>
-    <t>FC_NOTCH_DIFF_CF_EM_FIR</t>
-  </si>
-  <si>
-    <t>FC_NOTCH_DIFF_DM_FIR</t>
-  </si>
-  <si>
-    <t>FC_ENTITIES_NOTCH_DIFF_DM_FIR</t>
-  </si>
-  <si>
-    <t>FC_NOTCH_DIFF_CF_DM_FIR</t>
   </si>
 </sst>
 </file>
@@ -10875,10 +10794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3627"/>
+  <dimension ref="A1:A3600"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3597" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3599" sqref="D3599"/>
+    <sheetView tabSelected="1" topLeftCell="A3590" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3601" sqref="A3601:A3627"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28885,141 +28804,6 @@
     <row r="3600" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3600" s="3" t="s">
         <v>3398</v>
-      </c>
-    </row>
-    <row r="3601" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3601" s="3" t="s">
-        <v>3399</v>
-      </c>
-    </row>
-    <row r="3602" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3602" s="3" t="s">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="3603" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3603" s="3" t="s">
-        <v>3401</v>
-      </c>
-    </row>
-    <row r="3604" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3604" s="3" t="s">
-        <v>3402</v>
-      </c>
-    </row>
-    <row r="3605" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3605" s="3" t="s">
-        <v>3403</v>
-      </c>
-    </row>
-    <row r="3606" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3606" s="3" t="s">
-        <v>3404</v>
-      </c>
-    </row>
-    <row r="3607" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3607" s="3" t="s">
-        <v>3405</v>
-      </c>
-    </row>
-    <row r="3608" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3608" s="3" t="s">
-        <v>3406</v>
-      </c>
-    </row>
-    <row r="3609" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3609" s="3" t="s">
-        <v>3407</v>
-      </c>
-    </row>
-    <row r="3610" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3610" s="3" t="s">
-        <v>3408</v>
-      </c>
-    </row>
-    <row r="3611" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3611" s="3" t="s">
-        <v>3409</v>
-      </c>
-    </row>
-    <row r="3612" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3612" s="3" t="s">
-        <v>3410</v>
-      </c>
-    </row>
-    <row r="3613" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3613" s="3" t="s">
-        <v>3411</v>
-      </c>
-    </row>
-    <row r="3614" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3614" s="3" t="s">
-        <v>3412</v>
-      </c>
-    </row>
-    <row r="3615" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3615" s="3" t="s">
-        <v>3413</v>
-      </c>
-    </row>
-    <row r="3616" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3616" s="3" t="s">
-        <v>3414</v>
-      </c>
-    </row>
-    <row r="3617" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3617" s="3" t="s">
-        <v>3415</v>
-      </c>
-    </row>
-    <row r="3618" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3618" s="3" t="s">
-        <v>3416</v>
-      </c>
-    </row>
-    <row r="3619" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3619" s="3" t="s">
-        <v>3417</v>
-      </c>
-    </row>
-    <row r="3620" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3620" s="3" t="s">
-        <v>3418</v>
-      </c>
-    </row>
-    <row r="3621" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3621" s="3" t="s">
-        <v>3419</v>
-      </c>
-    </row>
-    <row r="3622" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3622" s="3" t="s">
-        <v>3420</v>
-      </c>
-    </row>
-    <row r="3623" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3623" s="3" t="s">
-        <v>3421</v>
-      </c>
-    </row>
-    <row r="3624" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3624" s="3" t="s">
-        <v>3422</v>
-      </c>
-    </row>
-    <row r="3625" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3625" s="3" t="s">
-        <v>3423</v>
-      </c>
-    </row>
-    <row r="3626" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3626" s="3" t="s">
-        <v>3424</v>
-      </c>
-    </row>
-    <row r="3627" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3627" s="3" t="s">
-        <v>3425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 12 and 13 Test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/fitchfieldID.xlsx
+++ b/src/test/resources/fitchfieldID.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3604" uniqueCount="3403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="3405">
   <si>
     <t>fitchFieldId</t>
   </si>
@@ -10247,6 +10247,12 @@
   </si>
   <si>
     <t>FC_MRKT_SECTOR_ALL_DESC</t>
+  </si>
+  <si>
+    <t>FC_SWIFT_CODES</t>
+  </si>
+  <si>
+    <t>FC_LEI</t>
   </si>
 </sst>
 </file>
@@ -10364,7 +10370,41 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -10908,10 +10948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3604"/>
+  <dimension ref="A1:A3606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3596" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3601" sqref="A3601"/>
+    <sheetView tabSelected="1" topLeftCell="A3590" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3605" sqref="F3605"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28940,77 +28980,99 @@
         <v>3402</v>
       </c>
     </row>
+    <row r="3605" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3605" s="3" t="s">
+        <v>3403</v>
+      </c>
+    </row>
+    <row r="3606" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3606" s="3" t="s">
+        <v>3404</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A3289"/>
   <conditionalFormatting sqref="A34">
+    <cfRule type="duplicateValues" dxfId="31" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2465:A2475">
+    <cfRule type="expression" dxfId="30" priority="37">
+      <formula>IF(FIND(" ",$E2465)&gt;0,TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="29" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2476:A2757">
+    <cfRule type="expression" dxfId="28" priority="24">
+      <formula>IF(FIND(" ",$E2476)&gt;0,TRUE,FALSE)</formula>
+    </cfRule>
     <cfRule type="duplicateValues" dxfId="27" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2465:A2475">
-    <cfRule type="expression" dxfId="26" priority="33">
-      <formula>IF(FIND(" ",$E2465)&gt;0,TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="A2994:A3082">
+    <cfRule type="expression" dxfId="26" priority="20">
+      <formula>IF(FIND(" ",$E2994)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="25" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2476:A2757">
-    <cfRule type="expression" dxfId="24" priority="20">
-      <formula>IF(FIND(" ",$E2476)&gt;0,TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="A3083:A3290">
+    <cfRule type="expression" dxfId="24" priority="18">
+      <formula>IF(FIND(" ",$E3083)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="23" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2994:A3082">
+  <conditionalFormatting sqref="A2212">
     <cfRule type="expression" dxfId="22" priority="16">
-      <formula>IF(FIND(" ",$E2994)&gt;0,TRUE,FALSE)</formula>
+      <formula>IF(FIND(" ",$E2212)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="duplicateValues" dxfId="21" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3083:A3290">
-    <cfRule type="expression" dxfId="20" priority="14">
-      <formula>IF(FIND(" ",$E3083)&gt;0,TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="19" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2212">
-    <cfRule type="expression" dxfId="18" priority="12">
-      <formula>IF(FIND(" ",$E2212)&gt;0,TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="17" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2211 A2758:A2983 A2986:A2993 A3291:A3415 A2213:A2464 A3590:A3600 A3605:A1048576">
-    <cfRule type="expression" dxfId="16" priority="83">
+  <conditionalFormatting sqref="A1:A2211 A2758:A2983 A2986:A2993 A3291:A3415 A2213:A2464 A3590:A3600 A3607:A1048576">
+    <cfRule type="expression" dxfId="20" priority="87">
       <formula>IF(FIND(" ",$E1)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="15" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3416:A3553">
-    <cfRule type="duplicateValues" dxfId="14" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3554:A3589">
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>IF(FIND(" ",$E3554)&gt;0,TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="16" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3601">
+    <cfRule type="expression" dxfId="15" priority="11">
+      <formula>IF(FIND(" ",$E3601)&gt;0,TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="14" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3602">
     <cfRule type="expression" dxfId="13" priority="9">
-      <formula>IF(FIND(" ",$E3554)&gt;0,TRUE,FALSE)</formula>
+      <formula>IF(FIND(" ",$E3602)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="duplicateValues" dxfId="12" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3601">
+  <conditionalFormatting sqref="A3603">
     <cfRule type="expression" dxfId="11" priority="7">
-      <formula>IF(FIND(" ",$E3601)&gt;0,TRUE,FALSE)</formula>
+      <formula>IF(FIND(" ",$E3603)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3602">
+  <conditionalFormatting sqref="A3604">
     <cfRule type="expression" dxfId="9" priority="5">
-      <formula>IF(FIND(" ",$E3602)&gt;0,TRUE,FALSE)</formula>
+      <formula>IF(FIND(" ",$E3604)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3603">
+  <conditionalFormatting sqref="A3605">
     <cfRule type="expression" dxfId="7" priority="3">
-      <formula>IF(FIND(" ",$E3603)&gt;0,TRUE,FALSE)</formula>
+      <formula>IF(FIND(" ",$E3605)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3604">
+  <conditionalFormatting sqref="A3606">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>IF(FIND(" ",$E3604)&gt;0,TRUE,FALSE)</formula>
+      <formula>IF(FIND(" ",$E3606)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>

</xml_diff>